<commit_message>
Completed Login module with dataprivider 06-07-2024
</commit_message>
<xml_diff>
--- a/src/resources/ExcelFile.xlsx
+++ b/src/resources/ExcelFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLoginsheet" sheetId="1" r:id="rId1"/>
@@ -31,22 +31,22 @@
     <t>adityapawar@yopmail.com</t>
   </si>
   <si>
+    <t>InvalidLoginEmail</t>
+  </si>
+  <si>
+    <t>aditya."gmail.</t>
+  </si>
+  <si>
+    <t>test"gmail</t>
+  </si>
+  <si>
+    <t>testgmail.com</t>
+  </si>
+  <si>
+    <t>testing@gmail</t>
+  </si>
+  <si>
     <t>rohan@yopmail.com</t>
-  </si>
-  <si>
-    <t>InvalidLoginEmail</t>
-  </si>
-  <si>
-    <t>aditya."gmail.</t>
-  </si>
-  <si>
-    <t>test"gmail</t>
-  </si>
-  <si>
-    <t>testgmail.com</t>
-  </si>
-  <si>
-    <t>testing@gmail</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -422,7 +422,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -450,27 +450,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Login module with dataprivider 07-07-2024
</commit_message>
<xml_diff>
--- a/src/resources/ExcelFile.xlsx
+++ b/src/resources/ExcelFile.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLoginsheet" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidLoginEmail" sheetId="2" r:id="rId2"/>
+    <sheet name="signupdata" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -47,6 +48,24 @@
   </si>
   <si>
     <t>rohan@yopmail.com</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>consumerEmail</t>
+  </si>
+  <si>
+    <t>aditya</t>
+  </si>
+  <si>
+    <t>Pawar</t>
+  </si>
+  <si>
+    <t>adityapawarsignup@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -385,7 +404,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -480,4 +499,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>